<commit_message>
My full data set
</commit_message>
<xml_diff>
--- a/data/raw_data/Min fisk.xlsx
+++ b/data/raw_data/Min fisk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birgitvingenekren/Documents/Master/MASTER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birgitvingenekren/Documents/Master/MASTER/Birgit_master/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AE5429-EB6D-8940-98D2-DED065661397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818B90CF-D6C5-0A47-8A70-28E50F6156E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{780D2175-496A-EA40-B69E-5FCAE97D8304}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{780D2175-496A-EA40-B69E-5FCAE97D8304}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1279,9 +1279,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1308,6 +1305,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1661,15 +1661,15 @@
   <dimension ref="A1:AX164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="10" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="10" customWidth="1"/>
@@ -12639,14 +12639,14 @@
       <c r="AL95" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="AQ95" s="21" t="s">
+      <c r="AQ95" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="AR95" s="21"/>
-      <c r="AS95" s="21"/>
-      <c r="AT95" s="21"/>
-      <c r="AU95" s="21"/>
-      <c r="AV95" s="21"/>
+      <c r="AR95" s="33"/>
+      <c r="AS95" s="33"/>
+      <c r="AT95" s="33"/>
+      <c r="AU95" s="33"/>
+      <c r="AV95" s="33"/>
     </row>
     <row r="96" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A96" s="9" t="s">
@@ -17510,7 +17510,7 @@
       <c r="V137" s="10">
         <v>1</v>
       </c>
-      <c r="W137" s="22" t="s">
+      <c r="W137" s="21" t="s">
         <v>72</v>
       </c>
       <c r="X137" s="10" t="s">
@@ -17744,7 +17744,7 @@
       <c r="V139" s="10">
         <v>2</v>
       </c>
-      <c r="W139" s="22" t="s">
+      <c r="W139" s="21" t="s">
         <v>63</v>
       </c>
       <c r="X139" s="10" t="s">
@@ -19920,13 +19920,13 @@
       <c r="F158" s="13">
         <v>44446</v>
       </c>
-      <c r="G158" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H158" s="24" t="s">
+      <c r="G158" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H158" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="I158" s="24" t="s">
+      <c r="I158" s="23" t="s">
         <v>48</v>
       </c>
       <c r="J158" s="10" t="s">
@@ -20019,17 +20019,17 @@
       </c>
     </row>
     <row r="159" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A159" s="25" t="s">
+      <c r="A159" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="B159" s="25">
+      <c r="B159" s="24">
         <v>1</v>
       </c>
       <c r="C159" s="10" t="str">
         <f t="shared" si="11"/>
         <v>30-35</v>
       </c>
-      <c r="D159" s="25" t="s">
+      <c r="D159" s="24" t="s">
         <v>38</v>
       </c>
       <c r="E159" s="10" t="s">
@@ -20041,7 +20041,7 @@
       <c r="G159" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H159" s="24" t="s">
+      <c r="H159" s="23" t="s">
         <v>66</v>
       </c>
       <c r="I159" s="10" t="s">
@@ -20050,16 +20050,16 @@
       <c r="J159" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="K159" s="26">
+      <c r="K159" s="25">
         <v>29</v>
       </c>
       <c r="L159" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M159" s="24">
+      <c r="M159" s="23">
         <v>295</v>
       </c>
-      <c r="N159" s="24">
+      <c r="N159" s="23">
         <v>301</v>
       </c>
       <c r="O159" s="10">
@@ -20074,7 +20074,7 @@
       <c r="R159" s="10">
         <v>300</v>
       </c>
-      <c r="S159" s="25" t="s">
+      <c r="S159" s="24" t="s">
         <v>41</v>
       </c>
       <c r="T159" s="10">
@@ -20083,13 +20083,13 @@
       <c r="U159" s="10">
         <v>242</v>
       </c>
-      <c r="V159" s="25">
+      <c r="V159" s="24">
         <v>2</v>
       </c>
       <c r="W159" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="X159" s="25" t="s">
+      <c r="X159" s="24" t="s">
         <v>43</v>
       </c>
       <c r="Y159" s="10" t="s">
@@ -20098,7 +20098,7 @@
       <c r="Z159" s="10">
         <v>1</v>
       </c>
-      <c r="AA159" s="25" t="s">
+      <c r="AA159" s="24" t="s">
         <v>43</v>
       </c>
       <c r="AB159" s="10" t="s">
@@ -20107,16 +20107,16 @@
       <c r="AC159" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AD159" s="25" t="s">
+      <c r="AD159" s="24" t="s">
         <v>58</v>
       </c>
       <c r="AE159" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="AF159" s="25" t="s">
+      <c r="AF159" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="AG159" s="24" t="s">
+      <c r="AG159" s="23" t="s">
         <v>82</v>
       </c>
       <c r="AH159" s="16" t="s">
@@ -20149,7 +20149,7 @@
       <c r="D160" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E160" s="25" t="s">
+      <c r="E160" s="24" t="s">
         <v>46</v>
       </c>
       <c r="F160" s="13">
@@ -20251,18 +20251,18 @@
       <c r="AL160" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="AM160" s="25"/>
-      <c r="AN160" s="25"/>
-      <c r="AO160" s="25"/>
-      <c r="AP160" s="25"/>
-      <c r="AQ160" s="25"/>
-      <c r="AR160" s="25"/>
-      <c r="AS160" s="25"/>
-      <c r="AT160" s="25"/>
-      <c r="AU160" s="25"/>
-      <c r="AV160" s="25"/>
-      <c r="AW160" s="25"/>
-      <c r="AX160" s="27"/>
+      <c r="AM160" s="24"/>
+      <c r="AN160" s="24"/>
+      <c r="AO160" s="24"/>
+      <c r="AP160" s="24"/>
+      <c r="AQ160" s="24"/>
+      <c r="AR160" s="24"/>
+      <c r="AS160" s="24"/>
+      <c r="AT160" s="24"/>
+      <c r="AU160" s="24"/>
+      <c r="AV160" s="24"/>
+      <c r="AW160" s="24"/>
+      <c r="AX160" s="26"/>
     </row>
     <row r="161" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A161" s="9" t="s">
@@ -20278,7 +20278,7 @@
       <c r="D161" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E161" s="25" t="s">
+      <c r="E161" s="24" t="s">
         <v>46</v>
       </c>
       <c r="F161" s="13">
@@ -20380,68 +20380,68 @@
       <c r="AL161" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="AM161" s="25"/>
-      <c r="AN161" s="25"/>
-      <c r="AO161" s="25"/>
-      <c r="AP161" s="25"/>
-      <c r="AQ161" s="25"/>
-      <c r="AR161" s="25"/>
-      <c r="AS161" s="25"/>
-      <c r="AT161" s="25"/>
-      <c r="AU161" s="25"/>
-      <c r="AV161" s="25"/>
-      <c r="AW161" s="25"/>
-      <c r="AX161" s="27"/>
+      <c r="AM161" s="24"/>
+      <c r="AN161" s="24"/>
+      <c r="AO161" s="24"/>
+      <c r="AP161" s="24"/>
+      <c r="AQ161" s="24"/>
+      <c r="AR161" s="24"/>
+      <c r="AS161" s="24"/>
+      <c r="AT161" s="24"/>
+      <c r="AU161" s="24"/>
+      <c r="AV161" s="24"/>
+      <c r="AW161" s="24"/>
+      <c r="AX161" s="26"/>
     </row>
     <row r="162" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A162" s="28" t="s">
+      <c r="A162" s="27" t="s">
         <v>334</v>
       </c>
-      <c r="B162" s="28"/>
-      <c r="C162" s="28"/>
-      <c r="D162" s="29"/>
+      <c r="B162" s="27"/>
+      <c r="C162" s="27"/>
+      <c r="D162" s="28"/>
       <c r="E162" s="8"/>
-      <c r="F162" s="30"/>
-      <c r="G162" s="29"/>
-      <c r="H162" s="29"/>
-      <c r="I162" s="29"/>
-      <c r="J162" s="29"/>
-      <c r="K162" s="29"/>
-      <c r="L162" s="29"/>
-      <c r="M162" s="29"/>
-      <c r="N162" s="29"/>
-      <c r="O162" s="29"/>
-      <c r="P162" s="29"/>
-      <c r="Q162" s="29"/>
-      <c r="R162" s="29"/>
-      <c r="S162" s="29"/>
-      <c r="T162" s="29"/>
-      <c r="U162" s="29"/>
-      <c r="V162" s="29"/>
-      <c r="W162" s="29"/>
-      <c r="X162" s="29"/>
-      <c r="Y162" s="29"/>
-      <c r="Z162" s="29"/>
-      <c r="AA162" s="29"/>
-      <c r="AB162" s="29"/>
-      <c r="AC162" s="29"/>
-      <c r="AD162" s="29"/>
-      <c r="AE162" s="29"/>
-      <c r="AF162" s="29"/>
-      <c r="AG162" s="29"/>
-      <c r="AH162" s="29"/>
-      <c r="AI162" s="28"/>
-      <c r="AJ162" s="31"/>
-      <c r="AK162" s="31"/>
+      <c r="F162" s="29"/>
+      <c r="G162" s="28"/>
+      <c r="H162" s="28"/>
+      <c r="I162" s="28"/>
+      <c r="J162" s="28"/>
+      <c r="K162" s="28"/>
+      <c r="L162" s="28"/>
+      <c r="M162" s="28"/>
+      <c r="N162" s="28"/>
+      <c r="O162" s="28"/>
+      <c r="P162" s="28"/>
+      <c r="Q162" s="28"/>
+      <c r="R162" s="28"/>
+      <c r="S162" s="28"/>
+      <c r="T162" s="28"/>
+      <c r="U162" s="28"/>
+      <c r="V162" s="28"/>
+      <c r="W162" s="28"/>
+      <c r="X162" s="28"/>
+      <c r="Y162" s="28"/>
+      <c r="Z162" s="28"/>
+      <c r="AA162" s="28"/>
+      <c r="AB162" s="28"/>
+      <c r="AC162" s="28"/>
+      <c r="AD162" s="28"/>
+      <c r="AE162" s="28"/>
+      <c r="AF162" s="28"/>
+      <c r="AG162" s="28"/>
+      <c r="AH162" s="28"/>
+      <c r="AI162" s="27"/>
+      <c r="AJ162" s="30"/>
+      <c r="AK162" s="30"/>
       <c r="AL162" s="8"/>
     </row>
     <row r="163" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A163" s="32" t="s">
+      <c r="A163" s="31" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="164" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A164" s="32" t="s">
+      <c r="A164" s="31" t="s">
         <v>334</v>
       </c>
     </row>

</xml_diff>